<commit_message>
Task #6386: update staff resource import files and views
</commit_message>
<xml_diff>
--- a/import_source/staff_resource_classic.xlsx
+++ b/import_source/staff_resource_classic.xlsx
@@ -11,10 +11,10 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$G$192</definedName>
-    <definedName name="staff_resources.classic" localSheetId="0">Sheet1!$C$15:$F$192</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$G$193</definedName>
+    <definedName name="staff_resources.classic" localSheetId="0">Sheet1!$C$16:$F$193</definedName>
   </definedNames>
-  <calcPr calcId="140000" concurrentCalc="0"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -26,7 +26,7 @@
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
 <connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <connection id="1" name="staff_resources.classic.txt" type="6" refreshedVersion="0" background="1" saveData="1">
-    <textPr fileType="mac" codePage="10000" sourceFile="Macintosh HD:Users:xiaochangfeng:Downloads:staff_resources.classic.txt" tab="0" comma="1">
+    <textPr fileType="mac" sourceFile="Macintosh HD:Users:xiaochangfeng:Downloads:staff_resources.classic.txt" tab="0" comma="1">
       <textFields count="3">
         <textField/>
         <textField/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="927" uniqueCount="383">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1098" uniqueCount="423">
   <si>
     <t>http://www6.slac.stanford.edu/about/organization.aspx</t>
   </si>
@@ -1187,6 +1187,126 @@
   </si>
   <si>
     <t>Women's Interchange at SLAC</t>
+  </si>
+  <si>
+    <t>Top Links</t>
+  </si>
+  <si>
+    <t>Top Links, Central Services</t>
+  </si>
+  <si>
+    <t>Top Links, Policies &amp; Procedures</t>
+  </si>
+  <si>
+    <t>Harvest Cafe Menu</t>
+  </si>
+  <si>
+    <t>http://www.stanford.edu/dept/rde/cgi-bin/slac/harvestcafe</t>
+  </si>
+  <si>
+    <t>Modern</t>
+  </si>
+  <si>
+    <t>New Employee Portal</t>
+  </si>
+  <si>
+    <t>https://www-internal.slac.stanford.edu/humanresources/training/NewEmployeePortal.aspx</t>
+  </si>
+  <si>
+    <t>SLAC Today</t>
+  </si>
+  <si>
+    <t>https://news.slac.stanford.edu/today/</t>
+  </si>
+  <si>
+    <t>Top Links, Safety &amp; Training</t>
+  </si>
+  <si>
+    <t>http://www-internal.slac.stanford.edu/websolutions/</t>
+  </si>
+  <si>
+    <t>https://slacportal.slac.stanford.edu/sites/esh/emergency/Pages/default.aspx</t>
+  </si>
+  <si>
+    <t>https://www-bis2.slac.stanford.edu//slaconly/training/</t>
+  </si>
+  <si>
+    <t>https://www-internal.slac.stanford.edu/humanresources/training/SLAC_Training_Assistance_Program.aspx</t>
+  </si>
+  <si>
+    <t>http://itservices.stanford.edu/service/techtraining/onlinetraining</t>
+  </si>
+  <si>
+    <t>http://www.stanford.edu/dept/dms/hrdata/eap/strp.html</t>
+  </si>
+  <si>
+    <t>https://www-internal.slac.stanford.edu/ocfo/bu/conferenceInfo.html</t>
+  </si>
+  <si>
+    <t>https://www-internal.slac.stanford.edu/ocfo/bu/PettyCashInformation.htm</t>
+  </si>
+  <si>
+    <t>http://www-group.slac.stanford.edu/ocfo/travel/documents/TravelPolicyandProcedure.pdf</t>
+  </si>
+  <si>
+    <t>Top Links, HR Services &amp; Benefits</t>
+  </si>
+  <si>
+    <t>https://www-internal.slac.stanford.edu/humanresources/employee-relations/default.aspx</t>
+  </si>
+  <si>
+    <t>https://www-internal.slac.stanford.edu/humanresources/general/winter-closure.aspx</t>
+  </si>
+  <si>
+    <t>https://www-internal.slac.stanford.edu/humanresources/international-services/</t>
+  </si>
+  <si>
+    <t>http://www2.slac.stanford.edu/lectures/</t>
+  </si>
+  <si>
+    <t>https://www-internal.slac.stanford.edu/humanresources/general/blood-drive.aspx</t>
+  </si>
+  <si>
+    <t>https://www.slac.stanford.edu/cgi-bin/meetingmaker/200512/webevent.cgi</t>
+  </si>
+  <si>
+    <t>HR Services &amp; Benefits, Life at SLAC</t>
+  </si>
+  <si>
+    <t>http://www.stanford.edu/dept/pe/cgi-bin/</t>
+  </si>
+  <si>
+    <t>http://www-project.slac.stanford.edu/wis/</t>
+  </si>
+  <si>
+    <t>http://www.interactions.org/</t>
+  </si>
+  <si>
+    <t>https://portal.slac.stanford.edu/info/esh/lessonslearned/SitePages/Home.aspx</t>
+  </si>
+  <si>
+    <t>Lessons Learned</t>
+  </si>
+  <si>
+    <t>http://www.lightsources.org/</t>
+  </si>
+  <si>
+    <t>http://transportation.stanford.edu/marguerite/MargueriteSched.shtml</t>
+  </si>
+  <si>
+    <t>http://www-project.slac.stanford.edu/rsbproject/</t>
+  </si>
+  <si>
+    <t>https://slacportal.slac.stanford.edu/</t>
+  </si>
+  <si>
+    <t>Stanford Maps</t>
+  </si>
+  <si>
+    <t>http://www.stanford.edu/dept/visitorinfo/plan/maps.html</t>
+  </si>
+  <si>
+    <t>http://www.symmetrymagazine.org/</t>
   </si>
 </sst>
 </file>
@@ -1810,10 +1930,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G192"/>
+  <dimension ref="A1:G221"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="D43" sqref="D43"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2008,9 +2129,8 @@
       <c r="D12" t="s">
         <v>322</v>
       </c>
-      <c r="G12" t="e">
-        <f>VLOOKUP(B12, Sheet2!$A$1:$B$65, 2, FALSE)</f>
-        <v>#N/A</v>
+      <c r="G12" t="s">
+        <v>383</v>
       </c>
     </row>
     <row r="13" spans="1:7">
@@ -2033,28 +2153,18 @@
         <v>13</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>334</v>
+        <v>388</v>
       </c>
       <c r="D14" t="s">
         <v>322</v>
-      </c>
-      <c r="E14" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="G14" t="e">
-        <f>VLOOKUP(B14, Sheet2!$A$1:$B$65, 2, FALSE)</f>
-        <v>#N/A</v>
       </c>
     </row>
     <row r="15" spans="1:7">
       <c r="A15">
         <v>14</v>
       </c>
-      <c r="B15" t="s">
-        <v>1</v>
-      </c>
-      <c r="C15" t="s">
-        <v>0</v>
+      <c r="B15" s="3" t="s">
+        <v>334</v>
       </c>
       <c r="D15" t="s">
         <v>322</v>
@@ -2072,10 +2182,10 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C16" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D16" t="s">
         <v>322</v>
@@ -2083,9 +2193,8 @@
       <c r="E16" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="G16" t="e">
-        <f>VLOOKUP(B16, Sheet2!$A$1:$B$65, 2, FALSE)</f>
-        <v>#N/A</v>
+      <c r="G16" t="s">
+        <v>383</v>
       </c>
     </row>
     <row r="17" spans="1:7">
@@ -2093,23 +2202,19 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C17" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D17" t="s">
         <v>322</v>
       </c>
-      <c r="E17" s="3" t="s">
-        <v>334</v>
-      </c>
-      <c r="F17" t="s">
-        <v>18</v>
-      </c>
-      <c r="G17" t="e">
-        <f>VLOOKUP(B17, Sheet2!$A$1:$B$65, 2, FALSE)</f>
-        <v>#N/A</v>
+      <c r="E17" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="G17" t="s">
+        <v>343</v>
       </c>
     </row>
     <row r="18" spans="1:7">
@@ -2117,16 +2222,16 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C18" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D18" t="s">
         <v>322</v>
       </c>
-      <c r="E18" t="s">
-        <v>5</v>
+      <c r="E18" s="3" t="s">
+        <v>334</v>
       </c>
       <c r="F18" t="s">
         <v>18</v>
@@ -2141,10 +2246,10 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C19" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D19" t="s">
         <v>322</v>
@@ -2155,9 +2260,8 @@
       <c r="F19" t="s">
         <v>18</v>
       </c>
-      <c r="G19" t="e">
-        <f>VLOOKUP(B19, Sheet2!$A$1:$B$65, 2, FALSE)</f>
-        <v>#N/A</v>
+      <c r="G19" t="s">
+        <v>346</v>
       </c>
     </row>
     <row r="20" spans="1:7">
@@ -2165,10 +2269,10 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C20" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D20" t="s">
         <v>322</v>
@@ -2189,10 +2293,10 @@
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C21" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D21" t="s">
         <v>322</v>
@@ -2213,10 +2317,10 @@
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C22" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D22" t="s">
         <v>322</v>
@@ -2237,16 +2341,16 @@
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C23" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D23" t="s">
         <v>322</v>
       </c>
-      <c r="E23" s="3" t="s">
-        <v>334</v>
+      <c r="E23" t="s">
+        <v>5</v>
       </c>
       <c r="F23" t="s">
         <v>18</v>
@@ -2261,16 +2365,16 @@
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C24" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="D24" t="s">
-        <v>18</v>
+        <v>322</v>
       </c>
       <c r="E24" s="3" t="s">
-        <v>17</v>
+        <v>334</v>
       </c>
       <c r="F24" t="s">
         <v>18</v>
@@ -2285,13 +2389,13 @@
         <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C25" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D25" t="s">
-        <v>322</v>
+        <v>18</v>
       </c>
       <c r="E25" s="3" t="s">
         <v>17</v>
@@ -2309,13 +2413,13 @@
         <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C26" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="D26" t="s">
-        <v>18</v>
+        <v>322</v>
       </c>
       <c r="E26" s="3" t="s">
         <v>17</v>
@@ -2333,13 +2437,13 @@
         <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C27" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D27" t="s">
-        <v>322</v>
+        <v>18</v>
       </c>
       <c r="E27" s="3" t="s">
         <v>17</v>
@@ -2357,13 +2461,13 @@
         <v>27</v>
       </c>
       <c r="B28" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C28" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D28" t="s">
-        <v>18</v>
+        <v>322</v>
       </c>
       <c r="E28" s="3" t="s">
         <v>17</v>
@@ -2381,10 +2485,10 @@
         <v>28</v>
       </c>
       <c r="B29" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C29" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D29" t="s">
         <v>18</v>
@@ -2405,13 +2509,13 @@
         <v>29</v>
       </c>
       <c r="B30" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C30" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D30" t="s">
-        <v>322</v>
+        <v>18</v>
       </c>
       <c r="E30" s="3" t="s">
         <v>17</v>
@@ -2429,10 +2533,10 @@
         <v>30</v>
       </c>
       <c r="B31" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C31" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D31" t="s">
         <v>322</v>
@@ -2453,16 +2557,16 @@
         <v>31</v>
       </c>
       <c r="B32" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C32" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D32" t="s">
         <v>322</v>
       </c>
       <c r="E32" s="3" t="s">
-        <v>34</v>
+        <v>17</v>
       </c>
       <c r="F32" t="s">
         <v>18</v>
@@ -2477,10 +2581,10 @@
         <v>32</v>
       </c>
       <c r="B33" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C33" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D33" t="s">
         <v>322</v>
@@ -2501,10 +2605,10 @@
         <v>33</v>
       </c>
       <c r="B34" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C34" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D34" t="s">
         <v>322</v>
@@ -2515,9 +2619,8 @@
       <c r="F34" t="s">
         <v>18</v>
       </c>
-      <c r="G34" t="e">
-        <f>VLOOKUP(B34, Sheet2!$A$1:$B$65, 2, FALSE)</f>
-        <v>#N/A</v>
+      <c r="G34" t="s">
+        <v>325</v>
       </c>
     </row>
     <row r="35" spans="1:7">
@@ -2525,10 +2628,10 @@
         <v>34</v>
       </c>
       <c r="B35" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C35" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D35" t="s">
         <v>322</v>
@@ -2536,9 +2639,12 @@
       <c r="E35" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="G35" t="str">
+      <c r="F35" t="s">
+        <v>18</v>
+      </c>
+      <c r="G35" t="e">
         <f>VLOOKUP(B35, Sheet2!$A$1:$B$65, 2, FALSE)</f>
-        <v>Central Services</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="36" spans="1:7">
@@ -2546,10 +2652,10 @@
         <v>35</v>
       </c>
       <c r="B36" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C36" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D36" t="s">
         <v>322</v>
@@ -2557,9 +2663,9 @@
       <c r="E36" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="G36" t="e">
+      <c r="G36" t="str">
         <f>VLOOKUP(B36, Sheet2!$A$1:$B$65, 2, FALSE)</f>
-        <v>#N/A</v>
+        <v>Central Services</v>
       </c>
     </row>
     <row r="37" spans="1:7">
@@ -2567,13 +2673,13 @@
         <v>36</v>
       </c>
       <c r="B37" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C37" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D37" t="s">
-        <v>18</v>
+        <v>322</v>
       </c>
       <c r="E37" s="3" t="s">
         <v>34</v>
@@ -2588,19 +2694,16 @@
         <v>37</v>
       </c>
       <c r="B38" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C38" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D38" t="s">
-        <v>322</v>
+        <v>18</v>
       </c>
       <c r="E38" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="F38" t="s">
-        <v>18</v>
+        <v>34</v>
       </c>
       <c r="G38" t="e">
         <f>VLOOKUP(B38, Sheet2!$A$1:$B$65, 2, FALSE)</f>
@@ -2612,10 +2715,10 @@
         <v>38</v>
       </c>
       <c r="B39" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C39" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D39" t="s">
         <v>322</v>
@@ -2636,10 +2739,10 @@
         <v>39</v>
       </c>
       <c r="B40" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C40" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D40" t="s">
         <v>322</v>
@@ -2660,16 +2763,16 @@
         <v>40</v>
       </c>
       <c r="B41" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C41" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D41" t="s">
-        <v>18</v>
+        <v>322</v>
       </c>
       <c r="E41" s="3" t="s">
-        <v>334</v>
+        <v>17</v>
       </c>
       <c r="F41" t="s">
         <v>18</v>
@@ -2684,16 +2787,19 @@
         <v>41</v>
       </c>
       <c r="B42" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C42" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D42" t="s">
         <v>18</v>
       </c>
-      <c r="E42" t="s">
-        <v>54</v>
+      <c r="E42" s="3" t="s">
+        <v>334</v>
+      </c>
+      <c r="F42" t="s">
+        <v>18</v>
       </c>
       <c r="G42" t="e">
         <f>VLOOKUP(B42, Sheet2!$A$1:$B$65, 2, FALSE)</f>
@@ -2705,10 +2811,10 @@
         <v>42</v>
       </c>
       <c r="B43" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C43" t="s">
-        <v>29</v>
+        <v>55</v>
       </c>
       <c r="D43" t="s">
         <v>18</v>
@@ -2726,10 +2832,10 @@
         <v>43</v>
       </c>
       <c r="B44" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C44" t="s">
-        <v>58</v>
+        <v>29</v>
       </c>
       <c r="D44" t="s">
         <v>18</v>
@@ -2747,10 +2853,10 @@
         <v>44</v>
       </c>
       <c r="B45" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C45" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="D45" t="s">
         <v>18</v>
@@ -2768,19 +2874,16 @@
         <v>45</v>
       </c>
       <c r="B46" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C46" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="D46" t="s">
-        <v>322</v>
-      </c>
-      <c r="E46" s="3" t="s">
-        <v>334</v>
-      </c>
-      <c r="F46" t="s">
-        <v>18</v>
+        <v>18</v>
+      </c>
+      <c r="E46" t="s">
+        <v>54</v>
       </c>
       <c r="G46" t="e">
         <f>VLOOKUP(B46, Sheet2!$A$1:$B$65, 2, FALSE)</f>
@@ -2792,16 +2895,16 @@
         <v>46</v>
       </c>
       <c r="B47" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C47" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="D47" t="s">
         <v>322</v>
       </c>
-      <c r="E47" t="s">
-        <v>63</v>
+      <c r="E47" s="3" t="s">
+        <v>334</v>
       </c>
       <c r="F47" t="s">
         <v>18</v>
@@ -2816,10 +2919,10 @@
         <v>47</v>
       </c>
       <c r="B48" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C48" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D48" t="s">
         <v>322</v>
@@ -2840,10 +2943,10 @@
         <v>48</v>
       </c>
       <c r="B49" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C49" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D49" t="s">
         <v>322</v>
@@ -2864,10 +2967,10 @@
         <v>49</v>
       </c>
       <c r="B50" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C50" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="D50" t="s">
         <v>322</v>
@@ -2888,10 +2991,10 @@
         <v>50</v>
       </c>
       <c r="B51" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C51" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="D51" t="s">
         <v>322</v>
@@ -2912,10 +3015,10 @@
         <v>51</v>
       </c>
       <c r="B52" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C52" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="D52" t="s">
         <v>322</v>
@@ -2936,10 +3039,10 @@
         <v>52</v>
       </c>
       <c r="B53" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C53" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="D53" t="s">
         <v>322</v>
@@ -2960,16 +3063,16 @@
         <v>53</v>
       </c>
       <c r="B54" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C54" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="D54" t="s">
         <v>322</v>
       </c>
-      <c r="E54" s="3" t="s">
-        <v>334</v>
+      <c r="E54" t="s">
+        <v>63</v>
       </c>
       <c r="F54" t="s">
         <v>18</v>
@@ -2984,16 +3087,16 @@
         <v>54</v>
       </c>
       <c r="B55" t="s">
-        <v>318</v>
+        <v>79</v>
       </c>
       <c r="C55" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="D55" t="s">
         <v>322</v>
       </c>
-      <c r="E55" t="s">
-        <v>79</v>
+      <c r="E55" s="3" t="s">
+        <v>334</v>
       </c>
       <c r="F55" t="s">
         <v>18</v>
@@ -3008,23 +3111,23 @@
         <v>55</v>
       </c>
       <c r="B56" t="s">
-        <v>82</v>
+        <v>318</v>
       </c>
       <c r="C56" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D56" t="s">
         <v>322</v>
       </c>
       <c r="E56" t="s">
-        <v>318</v>
+        <v>79</v>
       </c>
       <c r="F56" t="s">
         <v>18</v>
       </c>
-      <c r="G56" t="str">
+      <c r="G56" t="e">
         <f>VLOOKUP(B56, Sheet2!$A$1:$B$65, 2, FALSE)</f>
-        <v>Central Services</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="57" spans="1:7">
@@ -3032,23 +3135,22 @@
         <v>56</v>
       </c>
       <c r="B57" t="s">
-        <v>317</v>
+        <v>82</v>
       </c>
       <c r="C57" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="D57" t="s">
         <v>322</v>
       </c>
       <c r="E57" t="s">
-        <v>79</v>
+        <v>318</v>
       </c>
       <c r="F57" t="s">
         <v>18</v>
       </c>
-      <c r="G57" t="e">
-        <f>VLOOKUP(B57, Sheet2!$A$1:$B$65, 2, FALSE)</f>
-        <v>#N/A</v>
+      <c r="G57" t="s">
+        <v>384</v>
       </c>
     </row>
     <row r="58" spans="1:7">
@@ -3056,10 +3158,10 @@
         <v>57</v>
       </c>
       <c r="B58" t="s">
-        <v>85</v>
+        <v>317</v>
       </c>
       <c r="C58" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D58" t="s">
         <v>322</v>
@@ -3070,9 +3172,8 @@
       <c r="F58" t="s">
         <v>18</v>
       </c>
-      <c r="G58" t="e">
-        <f>VLOOKUP(B58, Sheet2!$A$1:$B$65, 2, FALSE)</f>
-        <v>#N/A</v>
+      <c r="G58" t="s">
+        <v>348</v>
       </c>
     </row>
     <row r="59" spans="1:7">
@@ -3080,13 +3181,13 @@
         <v>58</v>
       </c>
       <c r="B59" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C59" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="D59" t="s">
-        <v>18</v>
+        <v>322</v>
       </c>
       <c r="E59" t="s">
         <v>79</v>
@@ -3104,10 +3205,10 @@
         <v>59</v>
       </c>
       <c r="B60" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C60" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="D60" t="s">
         <v>18</v>
@@ -3128,16 +3229,16 @@
         <v>60</v>
       </c>
       <c r="B61" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C61" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="D61" t="s">
-        <v>322</v>
-      </c>
-      <c r="E61" s="3" t="s">
-        <v>334</v>
+        <v>18</v>
+      </c>
+      <c r="E61" t="s">
+        <v>79</v>
       </c>
       <c r="F61" t="s">
         <v>18</v>
@@ -3152,16 +3253,16 @@
         <v>61</v>
       </c>
       <c r="B62" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C62" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="D62" t="s">
         <v>322</v>
       </c>
-      <c r="E62" t="s">
-        <v>91</v>
+      <c r="E62" s="3" t="s">
+        <v>334</v>
       </c>
       <c r="F62" t="s">
         <v>18</v>
@@ -3176,10 +3277,10 @@
         <v>62</v>
       </c>
       <c r="B63" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C63" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="D63" t="s">
         <v>322</v>
@@ -3200,10 +3301,10 @@
         <v>63</v>
       </c>
       <c r="B64" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C64" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="D64" t="s">
         <v>322</v>
@@ -3224,16 +3325,16 @@
         <v>64</v>
       </c>
       <c r="B65" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C65" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="D65" t="s">
         <v>322</v>
       </c>
-      <c r="E65" s="3" t="s">
-        <v>334</v>
+      <c r="E65" t="s">
+        <v>91</v>
       </c>
       <c r="F65" t="s">
         <v>18</v>
@@ -3248,16 +3349,16 @@
         <v>65</v>
       </c>
       <c r="B66" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C66" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="D66" t="s">
         <v>322</v>
       </c>
-      <c r="E66" t="s">
-        <v>99</v>
+      <c r="E66" s="3" t="s">
+        <v>334</v>
       </c>
       <c r="F66" t="s">
         <v>18</v>
@@ -3272,10 +3373,10 @@
         <v>66</v>
       </c>
       <c r="B67" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C67" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="D67" t="s">
         <v>322</v>
@@ -3296,10 +3397,10 @@
         <v>67</v>
       </c>
       <c r="B68" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="C68" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="D68" t="s">
         <v>322</v>
@@ -3320,10 +3421,10 @@
         <v>68</v>
       </c>
       <c r="B69" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C69" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="D69" t="s">
         <v>322</v>
@@ -3344,16 +3445,16 @@
         <v>69</v>
       </c>
       <c r="B70" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C70" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="D70" t="s">
         <v>322</v>
       </c>
-      <c r="E70" s="3" t="s">
-        <v>334</v>
+      <c r="E70" t="s">
+        <v>99</v>
       </c>
       <c r="F70" t="s">
         <v>18</v>
@@ -3368,16 +3469,16 @@
         <v>70</v>
       </c>
       <c r="B71" t="s">
-        <v>65</v>
+        <v>109</v>
       </c>
       <c r="C71" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="D71" t="s">
         <v>322</v>
       </c>
-      <c r="E71" t="s">
-        <v>109</v>
+      <c r="E71" s="3" t="s">
+        <v>334</v>
       </c>
       <c r="F71" t="s">
         <v>18</v>
@@ -3392,10 +3493,10 @@
         <v>71</v>
       </c>
       <c r="B72" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="C72" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D72" t="s">
         <v>322</v>
@@ -3416,10 +3517,10 @@
         <v>72</v>
       </c>
       <c r="B73" t="s">
-        <v>113</v>
+        <v>69</v>
       </c>
       <c r="C73" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D73" t="s">
         <v>322</v>
@@ -3440,10 +3541,10 @@
         <v>73</v>
       </c>
       <c r="B74" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="C74" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="D74" t="s">
         <v>322</v>
@@ -3464,10 +3565,10 @@
         <v>74</v>
       </c>
       <c r="B75" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="C75" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="D75" t="s">
         <v>322</v>
@@ -3488,10 +3589,10 @@
         <v>75</v>
       </c>
       <c r="B76" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="C76" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="D76" t="s">
         <v>322</v>
@@ -3512,16 +3613,19 @@
         <v>76</v>
       </c>
       <c r="B77" t="s">
-        <v>316</v>
+        <v>119</v>
       </c>
       <c r="C77" t="s">
-        <v>83</v>
+        <v>118</v>
       </c>
       <c r="D77" t="s">
         <v>322</v>
       </c>
-      <c r="E77" s="1" t="s">
-        <v>324</v>
+      <c r="E77" t="s">
+        <v>109</v>
+      </c>
+      <c r="F77" t="s">
+        <v>18</v>
       </c>
       <c r="G77" t="e">
         <f>VLOOKUP(B77, Sheet2!$A$1:$B$65, 2, FALSE)</f>
@@ -3533,16 +3637,16 @@
         <v>77</v>
       </c>
       <c r="B78" t="s">
-        <v>121</v>
+        <v>316</v>
       </c>
       <c r="C78" t="s">
-        <v>120</v>
+        <v>83</v>
       </c>
       <c r="D78" t="s">
         <v>322</v>
       </c>
-      <c r="E78" t="s">
-        <v>316</v>
+      <c r="E78" s="1" t="s">
+        <v>324</v>
       </c>
       <c r="G78" t="e">
         <f>VLOOKUP(B78, Sheet2!$A$1:$B$65, 2, FALSE)</f>
@@ -3554,10 +3658,10 @@
         <v>78</v>
       </c>
       <c r="B79" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="C79" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="D79" t="s">
         <v>322</v>
@@ -3565,9 +3669,9 @@
       <c r="E79" t="s">
         <v>316</v>
       </c>
-      <c r="G79" t="str">
+      <c r="G79" t="e">
         <f>VLOOKUP(B79, Sheet2!$A$1:$B$65, 2, FALSE)</f>
-        <v>Safety &amp; Training</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="80" spans="1:7">
@@ -3575,10 +3679,10 @@
         <v>79</v>
       </c>
       <c r="B80" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="C80" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="D80" t="s">
         <v>322</v>
@@ -3586,9 +3690,9 @@
       <c r="E80" t="s">
         <v>316</v>
       </c>
-      <c r="G80" t="e">
+      <c r="G80" t="str">
         <f>VLOOKUP(B80, Sheet2!$A$1:$B$65, 2, FALSE)</f>
-        <v>#N/A</v>
+        <v>Safety &amp; Training</v>
       </c>
     </row>
     <row r="81" spans="1:7">
@@ -3596,10 +3700,10 @@
         <v>80</v>
       </c>
       <c r="B81" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="C81" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="D81" t="s">
         <v>322</v>
@@ -3607,9 +3711,8 @@
       <c r="E81" t="s">
         <v>316</v>
       </c>
-      <c r="G81" t="str">
-        <f>VLOOKUP(B81, Sheet2!$A$1:$B$65, 2, FALSE)</f>
-        <v>Safety &amp; Training</v>
+      <c r="G81" t="s">
+        <v>348</v>
       </c>
     </row>
     <row r="82" spans="1:7">
@@ -3617,10 +3720,10 @@
         <v>81</v>
       </c>
       <c r="B82" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="C82" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="D82" t="s">
         <v>322</v>
@@ -3628,9 +3731,8 @@
       <c r="E82" t="s">
         <v>316</v>
       </c>
-      <c r="G82" t="e">
-        <f>VLOOKUP(B82, Sheet2!$A$1:$B$65, 2, FALSE)</f>
-        <v>#N/A</v>
+      <c r="G82" t="s">
+        <v>393</v>
       </c>
     </row>
     <row r="83" spans="1:7">
@@ -3638,13 +3740,13 @@
         <v>82</v>
       </c>
       <c r="B83" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="C83" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="D83" t="s">
-        <v>18</v>
+        <v>322</v>
       </c>
       <c r="E83" t="s">
         <v>316</v>
@@ -3659,20 +3761,19 @@
         <v>83</v>
       </c>
       <c r="B84" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="C84" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="D84" t="s">
-        <v>322</v>
-      </c>
-      <c r="E84" s="1" t="s">
-        <v>325</v>
-      </c>
-      <c r="G84" t="e">
-        <f>VLOOKUP(B84, Sheet2!$A$1:$B$65, 2, FALSE)</f>
-        <v>#N/A</v>
+        <v>18</v>
+      </c>
+      <c r="E84" t="s">
+        <v>316</v>
+      </c>
+      <c r="G84" t="s">
+        <v>383</v>
       </c>
     </row>
     <row r="85" spans="1:7">
@@ -3680,10 +3781,10 @@
         <v>84</v>
       </c>
       <c r="B85" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="C85" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="D85" t="s">
         <v>322</v>
@@ -3701,10 +3802,10 @@
         <v>85</v>
       </c>
       <c r="B86" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="C86" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="D86" t="s">
         <v>322</v>
@@ -3712,9 +3813,8 @@
       <c r="E86" s="1" t="s">
         <v>325</v>
       </c>
-      <c r="G86" t="str">
-        <f>VLOOKUP(B86, Sheet2!$A$1:$B$65, 2, FALSE)</f>
-        <v>Central Services</v>
+      <c r="G86" t="s">
+        <v>342</v>
       </c>
     </row>
     <row r="87" spans="1:7">
@@ -3722,20 +3822,20 @@
         <v>86</v>
       </c>
       <c r="B87" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="C87" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="D87" t="s">
-        <v>18</v>
+        <v>322</v>
       </c>
       <c r="E87" s="1" t="s">
         <v>325</v>
       </c>
-      <c r="G87" t="e">
+      <c r="G87" t="str">
         <f>VLOOKUP(B87, Sheet2!$A$1:$B$65, 2, FALSE)</f>
-        <v>#N/A</v>
+        <v>Central Services</v>
       </c>
     </row>
     <row r="88" spans="1:7">
@@ -3743,10 +3843,10 @@
         <v>87</v>
       </c>
       <c r="B88" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="C88" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="D88" t="s">
         <v>18</v>
@@ -3764,10 +3864,10 @@
         <v>88</v>
       </c>
       <c r="B89" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="C89" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="D89" t="s">
         <v>18</v>
@@ -3775,9 +3875,8 @@
       <c r="E89" s="1" t="s">
         <v>325</v>
       </c>
-      <c r="G89" t="e">
-        <f>VLOOKUP(B89, Sheet2!$A$1:$B$65, 2, FALSE)</f>
-        <v>#N/A</v>
+      <c r="G89" t="s">
+        <v>383</v>
       </c>
     </row>
     <row r="90" spans="1:7">
@@ -3785,13 +3884,13 @@
         <v>89</v>
       </c>
       <c r="B90" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C90" t="s">
-        <v>8</v>
+        <v>142</v>
       </c>
       <c r="D90" t="s">
-        <v>322</v>
+        <v>18</v>
       </c>
       <c r="E90" s="1" t="s">
         <v>325</v>
@@ -3806,10 +3905,10 @@
         <v>90</v>
       </c>
       <c r="B91" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="C91" t="s">
-        <v>145</v>
+        <v>8</v>
       </c>
       <c r="D91" t="s">
         <v>322</v>
@@ -3827,20 +3926,20 @@
         <v>91</v>
       </c>
       <c r="B92" t="s">
-        <v>82</v>
+        <v>146</v>
       </c>
       <c r="C92" t="s">
-        <v>81</v>
+        <v>145</v>
       </c>
       <c r="D92" t="s">
         <v>322</v>
       </c>
-      <c r="E92" t="s">
-        <v>146</v>
-      </c>
-      <c r="G92" t="str">
+      <c r="E92" s="1" t="s">
+        <v>325</v>
+      </c>
+      <c r="G92" t="e">
         <f>VLOOKUP(B92, Sheet2!$A$1:$B$65, 2, FALSE)</f>
-        <v>Central Services</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="93" spans="1:7">
@@ -3848,20 +3947,20 @@
         <v>92</v>
       </c>
       <c r="B93" t="s">
-        <v>148</v>
+        <v>82</v>
       </c>
       <c r="C93" t="s">
-        <v>147</v>
+        <v>81</v>
       </c>
       <c r="D93" t="s">
         <v>322</v>
       </c>
-      <c r="E93" s="1" t="s">
-        <v>325</v>
-      </c>
-      <c r="G93" t="e">
+      <c r="E93" t="s">
+        <v>146</v>
+      </c>
+      <c r="G93" t="str">
         <f>VLOOKUP(B93, Sheet2!$A$1:$B$65, 2, FALSE)</f>
-        <v>#N/A</v>
+        <v>Central Services</v>
       </c>
     </row>
     <row r="94" spans="1:7">
@@ -3869,10 +3968,10 @@
         <v>93</v>
       </c>
       <c r="B94" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="C94" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="D94" t="s">
         <v>322</v>
@@ -3880,9 +3979,8 @@
       <c r="E94" s="1" t="s">
         <v>325</v>
       </c>
-      <c r="G94" t="e">
-        <f>VLOOKUP(B94, Sheet2!$A$1:$B$65, 2, FALSE)</f>
-        <v>#N/A</v>
+      <c r="G94" t="s">
+        <v>325</v>
       </c>
     </row>
     <row r="95" spans="1:7">
@@ -3890,10 +3988,10 @@
         <v>94</v>
       </c>
       <c r="B95" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="C95" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="D95" t="s">
         <v>322</v>
@@ -3901,9 +3999,8 @@
       <c r="E95" s="1" t="s">
         <v>325</v>
       </c>
-      <c r="G95" t="e">
-        <f>VLOOKUP(B95, Sheet2!$A$1:$B$65, 2, FALSE)</f>
-        <v>#N/A</v>
+      <c r="G95" t="s">
+        <v>383</v>
       </c>
     </row>
     <row r="96" spans="1:7">
@@ -3911,10 +4008,10 @@
         <v>95</v>
       </c>
       <c r="B96" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="C96" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="D96" t="s">
         <v>322</v>
@@ -3922,9 +4019,8 @@
       <c r="E96" s="1" t="s">
         <v>325</v>
       </c>
-      <c r="G96" t="e">
-        <f>VLOOKUP(B96, Sheet2!$A$1:$B$65, 2, FALSE)</f>
-        <v>#N/A</v>
+      <c r="G96" t="s">
+        <v>325</v>
       </c>
     </row>
     <row r="97" spans="1:7">
@@ -3932,10 +4028,10 @@
         <v>96</v>
       </c>
       <c r="B97" t="s">
-        <v>7</v>
+        <v>154</v>
       </c>
       <c r="C97" t="s">
-        <v>6</v>
+        <v>153</v>
       </c>
       <c r="D97" t="s">
         <v>322</v>
@@ -3953,16 +4049,16 @@
         <v>97</v>
       </c>
       <c r="B98" t="s">
-        <v>155</v>
+        <v>7</v>
       </c>
       <c r="C98" t="s">
-        <v>132</v>
+        <v>6</v>
       </c>
       <c r="D98" t="s">
         <v>322</v>
       </c>
-      <c r="E98" t="s">
-        <v>7</v>
+      <c r="E98" s="1" t="s">
+        <v>325</v>
       </c>
       <c r="G98" t="e">
         <f>VLOOKUP(B98, Sheet2!$A$1:$B$65, 2, FALSE)</f>
@@ -3974,13 +4070,13 @@
         <v>98</v>
       </c>
       <c r="B99" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="C99" t="s">
-        <v>156</v>
+        <v>132</v>
       </c>
       <c r="D99" t="s">
-        <v>18</v>
+        <v>322</v>
       </c>
       <c r="E99" t="s">
         <v>7</v>
@@ -3995,20 +4091,20 @@
         <v>99</v>
       </c>
       <c r="B100" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C100" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="D100" t="s">
-        <v>322</v>
-      </c>
-      <c r="E100" s="1" t="s">
-        <v>325</v>
-      </c>
-      <c r="G100" t="str">
+        <v>18</v>
+      </c>
+      <c r="E100" t="s">
+        <v>7</v>
+      </c>
+      <c r="G100" t="e">
         <f>VLOOKUP(B100, Sheet2!$A$1:$B$65, 2, FALSE)</f>
-        <v>Central Services</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="101" spans="1:7">
@@ -4016,20 +4112,20 @@
         <v>100</v>
       </c>
       <c r="B101" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="C101" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="D101" t="s">
-        <v>18</v>
-      </c>
-      <c r="E101" t="s">
-        <v>159</v>
+        <v>322</v>
+      </c>
+      <c r="E101" s="1" t="s">
+        <v>325</v>
       </c>
       <c r="G101" t="str">
         <f>VLOOKUP(B101, Sheet2!$A$1:$B$65, 2, FALSE)</f>
-        <v>Policies &amp; Procedures</v>
+        <v>Central Services</v>
       </c>
     </row>
     <row r="102" spans="1:7">
@@ -4037,20 +4133,19 @@
         <v>101</v>
       </c>
       <c r="B102" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="C102" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="D102" t="s">
-        <v>322</v>
-      </c>
-      <c r="E102" s="1" t="s">
-        <v>325</v>
-      </c>
-      <c r="G102" t="e">
-        <f>VLOOKUP(B102, Sheet2!$A$1:$B$65, 2, FALSE)</f>
-        <v>#N/A</v>
+        <v>18</v>
+      </c>
+      <c r="E102" t="s">
+        <v>159</v>
+      </c>
+      <c r="G102" t="s">
+        <v>385</v>
       </c>
     </row>
     <row r="103" spans="1:7">
@@ -4058,10 +4153,10 @@
         <v>102</v>
       </c>
       <c r="B103" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C103" t="s">
-        <v>12</v>
+        <v>162</v>
       </c>
       <c r="D103" t="s">
         <v>322</v>
@@ -4069,9 +4164,8 @@
       <c r="E103" s="1" t="s">
         <v>325</v>
       </c>
-      <c r="G103" t="e">
-        <f>VLOOKUP(B103, Sheet2!$A$1:$B$65, 2, FALSE)</f>
-        <v>#N/A</v>
+      <c r="G103" t="s">
+        <v>346</v>
       </c>
     </row>
     <row r="104" spans="1:7">
@@ -4079,10 +4173,10 @@
         <v>103</v>
       </c>
       <c r="B104" t="s">
-        <v>335</v>
+        <v>164</v>
       </c>
       <c r="C104" t="s">
-        <v>165</v>
+        <v>12</v>
       </c>
       <c r="D104" t="s">
         <v>322</v>
@@ -4100,16 +4194,16 @@
         <v>104</v>
       </c>
       <c r="B105" t="s">
-        <v>167</v>
+        <v>335</v>
       </c>
       <c r="C105" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="D105" t="s">
         <v>322</v>
       </c>
-      <c r="E105" t="s">
-        <v>335</v>
+      <c r="E105" s="1" t="s">
+        <v>325</v>
       </c>
       <c r="G105" t="e">
         <f>VLOOKUP(B105, Sheet2!$A$1:$B$65, 2, FALSE)</f>
@@ -4121,10 +4215,10 @@
         <v>105</v>
       </c>
       <c r="B106" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="C106" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="D106" t="s">
         <v>322</v>
@@ -4142,10 +4236,10 @@
         <v>106</v>
       </c>
       <c r="B107" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="C107" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="D107" t="s">
         <v>322</v>
@@ -4163,20 +4257,20 @@
         <v>107</v>
       </c>
       <c r="B108" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="C108" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="D108" t="s">
         <v>322</v>
       </c>
-      <c r="E108" s="1" t="s">
-        <v>325</v>
-      </c>
-      <c r="G108" t="str">
+      <c r="E108" t="s">
+        <v>335</v>
+      </c>
+      <c r="G108" t="e">
         <f>VLOOKUP(B108, Sheet2!$A$1:$B$65, 2, FALSE)</f>
-        <v>Safety &amp; Training</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="109" spans="1:7">
@@ -4184,10 +4278,10 @@
         <v>108</v>
       </c>
       <c r="B109" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="C109" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="D109" t="s">
         <v>322</v>
@@ -4195,9 +4289,9 @@
       <c r="E109" s="1" t="s">
         <v>325</v>
       </c>
-      <c r="G109" t="e">
+      <c r="G109" t="str">
         <f>VLOOKUP(B109, Sheet2!$A$1:$B$65, 2, FALSE)</f>
-        <v>#N/A</v>
+        <v>Safety &amp; Training</v>
       </c>
     </row>
     <row r="110" spans="1:7">
@@ -4205,10 +4299,10 @@
         <v>109</v>
       </c>
       <c r="B110" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="C110" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="D110" t="s">
         <v>322</v>
@@ -4226,10 +4320,10 @@
         <v>110</v>
       </c>
       <c r="B111" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="C111" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="D111" t="s">
         <v>322</v>
@@ -4247,20 +4341,20 @@
         <v>111</v>
       </c>
       <c r="B112" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="C112" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="D112" t="s">
-        <v>18</v>
+        <v>322</v>
       </c>
       <c r="E112" s="1" t="s">
         <v>325</v>
       </c>
-      <c r="G112" t="str">
+      <c r="G112" t="e">
         <f>VLOOKUP(B112, Sheet2!$A$1:$B$65, 2, FALSE)</f>
-        <v>Central Services</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="113" spans="1:7">
@@ -4268,10 +4362,10 @@
         <v>112</v>
       </c>
       <c r="B113" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="C113" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="D113" t="s">
         <v>18</v>
@@ -4279,9 +4373,9 @@
       <c r="E113" s="1" t="s">
         <v>325</v>
       </c>
-      <c r="G113" t="e">
+      <c r="G113" t="str">
         <f>VLOOKUP(B113, Sheet2!$A$1:$B$65, 2, FALSE)</f>
-        <v>#N/A</v>
+        <v>Central Services</v>
       </c>
     </row>
     <row r="114" spans="1:7">
@@ -4289,10 +4383,10 @@
         <v>113</v>
       </c>
       <c r="B114" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="C114" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="D114" t="s">
         <v>18</v>
@@ -4300,9 +4394,9 @@
       <c r="E114" s="1" t="s">
         <v>325</v>
       </c>
-      <c r="G114" t="str">
+      <c r="G114" t="e">
         <f>VLOOKUP(B114, Sheet2!$A$1:$B$65, 2, FALSE)</f>
-        <v>Central Services</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="115" spans="1:7">
@@ -4310,10 +4404,10 @@
         <v>114</v>
       </c>
       <c r="B115" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="C115" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="D115" t="s">
         <v>18</v>
@@ -4321,9 +4415,9 @@
       <c r="E115" s="1" t="s">
         <v>325</v>
       </c>
-      <c r="G115" t="e">
+      <c r="G115" t="str">
         <f>VLOOKUP(B115, Sheet2!$A$1:$B$65, 2, FALSE)</f>
-        <v>#N/A</v>
+        <v>Central Services</v>
       </c>
     </row>
     <row r="116" spans="1:7">
@@ -4331,20 +4425,20 @@
         <v>115</v>
       </c>
       <c r="B116" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="C116" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="D116" t="s">
-        <v>322</v>
+        <v>18</v>
       </c>
       <c r="E116" s="1" t="s">
         <v>325</v>
       </c>
-      <c r="G116" t="str">
+      <c r="G116" t="e">
         <f>VLOOKUP(B116, Sheet2!$A$1:$B$65, 2, FALSE)</f>
-        <v>Central Services</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="117" spans="1:7">
@@ -4352,20 +4446,20 @@
         <v>116</v>
       </c>
       <c r="B117" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="C117" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="D117" t="s">
-        <v>18</v>
+        <v>322</v>
       </c>
       <c r="E117" s="1" t="s">
         <v>325</v>
       </c>
-      <c r="G117" t="e">
+      <c r="G117" t="str">
         <f>VLOOKUP(B117, Sheet2!$A$1:$B$65, 2, FALSE)</f>
-        <v>#N/A</v>
+        <v>Central Services</v>
       </c>
     </row>
     <row r="118" spans="1:7">
@@ -4373,13 +4467,13 @@
         <v>117</v>
       </c>
       <c r="B118" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="C118" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="D118" t="s">
-        <v>322</v>
+        <v>18</v>
       </c>
       <c r="E118" s="1" t="s">
         <v>325</v>
@@ -4394,13 +4488,13 @@
         <v>118</v>
       </c>
       <c r="B119" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="C119" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="D119" t="s">
-        <v>18</v>
+        <v>322</v>
       </c>
       <c r="E119" s="1" t="s">
         <v>325</v>
@@ -4415,13 +4509,13 @@
         <v>119</v>
       </c>
       <c r="B120" t="s">
-        <v>336</v>
+        <v>195</v>
       </c>
       <c r="C120" t="s">
-        <v>165</v>
+        <v>194</v>
       </c>
       <c r="D120" t="s">
-        <v>322</v>
+        <v>18</v>
       </c>
       <c r="E120" s="1" t="s">
         <v>325</v>
@@ -4436,16 +4530,16 @@
         <v>120</v>
       </c>
       <c r="B121" t="s">
-        <v>167</v>
+        <v>336</v>
       </c>
       <c r="C121" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="D121" t="s">
         <v>322</v>
       </c>
-      <c r="E121" t="s">
-        <v>336</v>
+      <c r="E121" s="1" t="s">
+        <v>325</v>
       </c>
       <c r="G121" t="e">
         <f>VLOOKUP(B121, Sheet2!$A$1:$B$65, 2, FALSE)</f>
@@ -4457,10 +4551,10 @@
         <v>121</v>
       </c>
       <c r="B122" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="C122" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="D122" t="s">
         <v>322</v>
@@ -4478,10 +4572,10 @@
         <v>122</v>
       </c>
       <c r="B123" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="C123" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="D123" t="s">
         <v>322</v>
@@ -4499,20 +4593,20 @@
         <v>123</v>
       </c>
       <c r="B124" t="s">
-        <v>197</v>
+        <v>171</v>
       </c>
       <c r="C124" t="s">
-        <v>196</v>
+        <v>170</v>
       </c>
       <c r="D124" t="s">
-        <v>18</v>
-      </c>
-      <c r="E124" s="1" t="s">
-        <v>325</v>
-      </c>
-      <c r="G124" t="str">
+        <v>322</v>
+      </c>
+      <c r="E124" t="s">
+        <v>336</v>
+      </c>
+      <c r="G124" t="e">
         <f>VLOOKUP(B124, Sheet2!$A$1:$B$65, 2, FALSE)</f>
-        <v>Central Services</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="125" spans="1:7">
@@ -4520,10 +4614,10 @@
         <v>124</v>
       </c>
       <c r="B125" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="C125" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="D125" t="s">
         <v>18</v>
@@ -4531,9 +4625,9 @@
       <c r="E125" s="1" t="s">
         <v>325</v>
       </c>
-      <c r="G125" t="e">
+      <c r="G125" t="str">
         <f>VLOOKUP(B125, Sheet2!$A$1:$B$65, 2, FALSE)</f>
-        <v>#N/A</v>
+        <v>Central Services</v>
       </c>
     </row>
     <row r="126" spans="1:7">
@@ -4541,10 +4635,10 @@
         <v>125</v>
       </c>
       <c r="B126" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="C126" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="D126" t="s">
         <v>18</v>
@@ -4562,20 +4656,19 @@
         <v>126</v>
       </c>
       <c r="B127" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="C127" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="D127" t="s">
-        <v>322</v>
+        <v>18</v>
       </c>
       <c r="E127" s="1" t="s">
         <v>325</v>
       </c>
-      <c r="G127" t="e">
-        <f>VLOOKUP(B127, Sheet2!$A$1:$B$65, 2, FALSE)</f>
-        <v>#N/A</v>
+      <c r="G127" t="s">
+        <v>383</v>
       </c>
     </row>
     <row r="128" spans="1:7">
@@ -4583,10 +4676,10 @@
         <v>127</v>
       </c>
       <c r="B128" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="C128" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="D128" t="s">
         <v>322</v>
@@ -4594,9 +4687,8 @@
       <c r="E128" s="1" t="s">
         <v>325</v>
       </c>
-      <c r="G128" t="e">
-        <f>VLOOKUP(B128, Sheet2!$A$1:$B$65, 2, FALSE)</f>
-        <v>#N/A</v>
+      <c r="G128" t="s">
+        <v>325</v>
       </c>
     </row>
     <row r="129" spans="1:7">
@@ -4604,20 +4696,19 @@
         <v>128</v>
       </c>
       <c r="B129" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="C129" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="D129" t="s">
-        <v>18</v>
+        <v>322</v>
       </c>
       <c r="E129" s="1" t="s">
         <v>325</v>
       </c>
-      <c r="G129" t="e">
-        <f>VLOOKUP(B129, Sheet2!$A$1:$B$65, 2, FALSE)</f>
-        <v>#N/A</v>
+      <c r="G129" t="s">
+        <v>383</v>
       </c>
     </row>
     <row r="130" spans="1:7">
@@ -4625,13 +4716,13 @@
         <v>129</v>
       </c>
       <c r="B130" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="C130" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="D130" t="s">
-        <v>322</v>
+        <v>18</v>
       </c>
       <c r="E130" s="1" t="s">
         <v>325</v>
@@ -4646,13 +4737,13 @@
         <v>130</v>
       </c>
       <c r="B131" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="C131" t="s">
-        <v>140</v>
+        <v>208</v>
       </c>
       <c r="D131" t="s">
-        <v>18</v>
+        <v>322</v>
       </c>
       <c r="E131" s="1" t="s">
         <v>325</v>
@@ -4667,13 +4758,13 @@
         <v>131</v>
       </c>
       <c r="B132" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="C132" t="s">
-        <v>211</v>
+        <v>140</v>
       </c>
       <c r="D132" t="s">
-        <v>322</v>
+        <v>18</v>
       </c>
       <c r="E132" s="1" t="s">
         <v>325</v>
@@ -4688,10 +4779,10 @@
         <v>132</v>
       </c>
       <c r="B133" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="C133" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="D133" t="s">
         <v>322</v>
@@ -4709,20 +4800,19 @@
         <v>133</v>
       </c>
       <c r="B134" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C134" t="s">
-        <v>68</v>
+        <v>213</v>
       </c>
       <c r="D134" t="s">
         <v>322</v>
       </c>
       <c r="E134" s="1" t="s">
-        <v>326</v>
-      </c>
-      <c r="G134" t="e">
-        <f>VLOOKUP(B134, Sheet2!$A$1:$B$65, 2, FALSE)</f>
-        <v>#N/A</v>
+        <v>325</v>
+      </c>
+      <c r="G134" t="s">
+        <v>383</v>
       </c>
     </row>
     <row r="135" spans="1:7">
@@ -4730,10 +4820,10 @@
         <v>134</v>
       </c>
       <c r="B135" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C135" t="s">
-        <v>111</v>
+        <v>68</v>
       </c>
       <c r="D135" t="s">
         <v>322</v>
@@ -4751,13 +4841,13 @@
         <v>135</v>
       </c>
       <c r="B136" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="C136" t="s">
-        <v>217</v>
+        <v>111</v>
       </c>
       <c r="D136" t="s">
-        <v>18</v>
+        <v>322</v>
       </c>
       <c r="E136" s="1" t="s">
         <v>326</v>
@@ -4772,10 +4862,10 @@
         <v>136</v>
       </c>
       <c r="B137" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="C137" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="D137" t="s">
         <v>18</v>
@@ -4793,10 +4883,10 @@
         <v>137</v>
       </c>
       <c r="B138" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="C138" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="D138" t="s">
         <v>18</v>
@@ -4814,20 +4904,20 @@
         <v>138</v>
       </c>
       <c r="B139" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="C139" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="D139" t="s">
-        <v>322</v>
+        <v>18</v>
       </c>
       <c r="E139" s="1" t="s">
-        <v>327</v>
-      </c>
-      <c r="G139" t="str">
+        <v>326</v>
+      </c>
+      <c r="G139" t="e">
         <f>VLOOKUP(B139, Sheet2!$A$1:$B$65, 2, FALSE)</f>
-        <v>Policies &amp; Procedures</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="140" spans="1:7">
@@ -4835,20 +4925,20 @@
         <v>139</v>
       </c>
       <c r="B140" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="C140" t="s">
-        <v>182</v>
+        <v>223</v>
       </c>
       <c r="D140" t="s">
-        <v>18</v>
+        <v>322</v>
       </c>
       <c r="E140" s="1" t="s">
         <v>327</v>
       </c>
-      <c r="G140" t="e">
+      <c r="G140" t="str">
         <f>VLOOKUP(B140, Sheet2!$A$1:$B$65, 2, FALSE)</f>
-        <v>#N/A</v>
+        <v>Policies &amp; Procedures</v>
       </c>
     </row>
     <row r="141" spans="1:7">
@@ -4856,10 +4946,10 @@
         <v>140</v>
       </c>
       <c r="B141" t="s">
-        <v>193</v>
+        <v>225</v>
       </c>
       <c r="C141" t="s">
-        <v>194</v>
+        <v>182</v>
       </c>
       <c r="D141" t="s">
         <v>18</v>
@@ -4877,20 +4967,20 @@
         <v>141</v>
       </c>
       <c r="B142" t="s">
-        <v>227</v>
+        <v>193</v>
       </c>
       <c r="C142" t="s">
-        <v>226</v>
+        <v>194</v>
       </c>
       <c r="D142" t="s">
-        <v>322</v>
+        <v>18</v>
       </c>
       <c r="E142" s="1" t="s">
         <v>327</v>
       </c>
-      <c r="G142" t="str">
+      <c r="G142" t="e">
         <f>VLOOKUP(B142, Sheet2!$A$1:$B$65, 2, FALSE)</f>
-        <v>Policies &amp; Procedures</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="143" spans="1:7">
@@ -4898,20 +4988,20 @@
         <v>142</v>
       </c>
       <c r="B143" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="C143" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="D143" t="s">
-        <v>18</v>
-      </c>
-      <c r="E143" s="2" t="s">
-        <v>328</v>
-      </c>
-      <c r="G143" t="e">
+        <v>322</v>
+      </c>
+      <c r="E143" s="1" t="s">
+        <v>327</v>
+      </c>
+      <c r="G143" t="str">
         <f>VLOOKUP(B143, Sheet2!$A$1:$B$65, 2, FALSE)</f>
-        <v>#N/A</v>
+        <v>Policies &amp; Procedures</v>
       </c>
     </row>
     <row r="144" spans="1:7">
@@ -4919,10 +5009,10 @@
         <v>143</v>
       </c>
       <c r="B144" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="C144" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="D144" t="s">
         <v>18</v>
@@ -4930,9 +5020,8 @@
       <c r="E144" s="2" t="s">
         <v>328</v>
       </c>
-      <c r="G144" t="e">
-        <f>VLOOKUP(B144, Sheet2!$A$1:$B$65, 2, FALSE)</f>
-        <v>#N/A</v>
+      <c r="G144" t="s">
+        <v>344</v>
       </c>
     </row>
     <row r="145" spans="1:7">
@@ -4940,20 +5029,19 @@
         <v>144</v>
       </c>
       <c r="B145" t="s">
-        <v>315</v>
+        <v>231</v>
       </c>
       <c r="C145" t="s">
-        <v>124</v>
+        <v>230</v>
       </c>
       <c r="D145" t="s">
-        <v>322</v>
-      </c>
-      <c r="E145" s="1" t="s">
-        <v>329</v>
-      </c>
-      <c r="G145" t="e">
-        <f>VLOOKUP(B145, Sheet2!$A$1:$B$65, 2, FALSE)</f>
-        <v>#N/A</v>
+        <v>18</v>
+      </c>
+      <c r="E145" s="2" t="s">
+        <v>328</v>
+      </c>
+      <c r="G145" t="s">
+        <v>344</v>
       </c>
     </row>
     <row r="146" spans="1:7">
@@ -4961,10 +5049,10 @@
         <v>145</v>
       </c>
       <c r="B146" t="s">
-        <v>233</v>
+        <v>315</v>
       </c>
       <c r="C146" t="s">
-        <v>232</v>
+        <v>124</v>
       </c>
       <c r="D146" t="s">
         <v>322</v>
@@ -4982,10 +5070,10 @@
         <v>146</v>
       </c>
       <c r="B147" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="C147" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="D147" t="s">
         <v>322</v>
@@ -4993,9 +5081,8 @@
       <c r="E147" s="1" t="s">
         <v>329</v>
       </c>
-      <c r="G147" t="e">
-        <f>VLOOKUP(B147, Sheet2!$A$1:$B$65, 2, FALSE)</f>
-        <v>#N/A</v>
+      <c r="G147" t="s">
+        <v>348</v>
       </c>
     </row>
     <row r="148" spans="1:7">
@@ -5003,7 +5090,10 @@
         <v>147</v>
       </c>
       <c r="B148" t="s">
-        <v>236</v>
+        <v>235</v>
+      </c>
+      <c r="C148" t="s">
+        <v>234</v>
       </c>
       <c r="D148" t="s">
         <v>322</v>
@@ -5021,20 +5111,17 @@
         <v>148</v>
       </c>
       <c r="B149" t="s">
-        <v>238</v>
-      </c>
-      <c r="C149" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="D149" t="s">
         <v>322</v>
       </c>
-      <c r="E149" t="s">
-        <v>236</v>
-      </c>
-      <c r="G149" t="str">
+      <c r="E149" s="1" t="s">
+        <v>329</v>
+      </c>
+      <c r="G149" t="e">
         <f>VLOOKUP(B149, Sheet2!$A$1:$B$65, 2, FALSE)</f>
-        <v>HR Services &amp; Benefits</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="150" spans="1:7">
@@ -5042,10 +5129,10 @@
         <v>149</v>
       </c>
       <c r="B150" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="C150" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="D150" t="s">
         <v>322</v>
@@ -5053,9 +5140,8 @@
       <c r="E150" t="s">
         <v>236</v>
       </c>
-      <c r="G150" t="str">
-        <f>VLOOKUP(B150, Sheet2!$A$1:$B$65, 2, FALSE)</f>
-        <v>Safety &amp; Training</v>
+      <c r="G150" t="s">
+        <v>410</v>
       </c>
     </row>
     <row r="151" spans="1:7">
@@ -5063,10 +5149,10 @@
         <v>150</v>
       </c>
       <c r="B151" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="C151" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="D151" t="s">
         <v>322</v>
@@ -5084,10 +5170,10 @@
         <v>151</v>
       </c>
       <c r="B152" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="C152" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="D152" t="s">
         <v>322</v>
@@ -5095,9 +5181,9 @@
       <c r="E152" t="s">
         <v>236</v>
       </c>
-      <c r="G152" t="e">
+      <c r="G152" t="str">
         <f>VLOOKUP(B152, Sheet2!$A$1:$B$65, 2, FALSE)</f>
-        <v>#N/A</v>
+        <v>Safety &amp; Training</v>
       </c>
     </row>
     <row r="153" spans="1:7">
@@ -5105,10 +5191,10 @@
         <v>152</v>
       </c>
       <c r="B153" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="C153" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="D153" t="s">
         <v>322</v>
@@ -5126,16 +5212,16 @@
         <v>153</v>
       </c>
       <c r="B154" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="C154" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="D154" t="s">
         <v>322</v>
       </c>
       <c r="E154" t="s">
-        <v>146</v>
+        <v>236</v>
       </c>
       <c r="G154" t="e">
         <f>VLOOKUP(B154, Sheet2!$A$1:$B$65, 2, FALSE)</f>
@@ -5147,16 +5233,16 @@
         <v>154</v>
       </c>
       <c r="B155" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="C155" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="D155" t="s">
         <v>322</v>
       </c>
       <c r="E155" t="s">
-        <v>249</v>
+        <v>146</v>
       </c>
       <c r="G155" t="e">
         <f>VLOOKUP(B155, Sheet2!$A$1:$B$65, 2, FALSE)</f>
@@ -5168,16 +5254,16 @@
         <v>155</v>
       </c>
       <c r="B156" t="s">
-        <v>247</v>
+        <v>251</v>
       </c>
       <c r="C156" t="s">
-        <v>145</v>
+        <v>250</v>
       </c>
       <c r="D156" t="s">
         <v>322</v>
       </c>
       <c r="E156" t="s">
-        <v>146</v>
+        <v>249</v>
       </c>
       <c r="G156" t="e">
         <f>VLOOKUP(B156, Sheet2!$A$1:$B$65, 2, FALSE)</f>
@@ -5189,10 +5275,10 @@
         <v>156</v>
       </c>
       <c r="B157" t="s">
-        <v>253</v>
+        <v>247</v>
       </c>
       <c r="C157" t="s">
-        <v>252</v>
+        <v>145</v>
       </c>
       <c r="D157" t="s">
         <v>322</v>
@@ -5210,10 +5296,10 @@
         <v>157</v>
       </c>
       <c r="B158" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="C158" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="D158" t="s">
         <v>322</v>
@@ -5231,10 +5317,10 @@
         <v>158</v>
       </c>
       <c r="B159" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="C159" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="D159" t="s">
         <v>322</v>
@@ -5252,10 +5338,10 @@
         <v>159</v>
       </c>
       <c r="B160" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="C160" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="D160" t="s">
         <v>322</v>
@@ -5273,16 +5359,16 @@
         <v>160</v>
       </c>
       <c r="B161" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="C161" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="D161" t="s">
         <v>322</v>
       </c>
       <c r="E161" t="s">
-        <v>259</v>
+        <v>146</v>
       </c>
       <c r="G161" t="e">
         <f>VLOOKUP(B161, Sheet2!$A$1:$B$65, 2, FALSE)</f>
@@ -5294,16 +5380,16 @@
         <v>161</v>
       </c>
       <c r="B162" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="C162" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="D162" t="s">
         <v>322</v>
       </c>
       <c r="E162" t="s">
-        <v>146</v>
+        <v>259</v>
       </c>
       <c r="G162" t="e">
         <f>VLOOKUP(B162, Sheet2!$A$1:$B$65, 2, FALSE)</f>
@@ -5315,10 +5401,10 @@
         <v>162</v>
       </c>
       <c r="B163" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="C163" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="D163" t="s">
         <v>322</v>
@@ -5326,9 +5412,9 @@
       <c r="E163" t="s">
         <v>146</v>
       </c>
-      <c r="G163" t="str">
+      <c r="G163" t="e">
         <f>VLOOKUP(B163, Sheet2!$A$1:$B$65, 2, FALSE)</f>
-        <v>Helpful Resources</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="164" spans="1:7">
@@ -5336,7 +5422,10 @@
         <v>163</v>
       </c>
       <c r="B164" t="s">
-        <v>337</v>
+        <v>265</v>
+      </c>
+      <c r="C164" t="s">
+        <v>264</v>
       </c>
       <c r="D164" t="s">
         <v>322</v>
@@ -5344,9 +5433,9 @@
       <c r="E164" t="s">
         <v>146</v>
       </c>
-      <c r="G164" t="e">
+      <c r="G164" t="str">
         <f>VLOOKUP(B164, Sheet2!$A$1:$B$65, 2, FALSE)</f>
-        <v>#N/A</v>
+        <v>Helpful Resources</v>
       </c>
     </row>
     <row r="165" spans="1:7">
@@ -5354,16 +5443,13 @@
         <v>164</v>
       </c>
       <c r="B165" t="s">
-        <v>268</v>
-      </c>
-      <c r="C165" t="s">
-        <v>267</v>
+        <v>337</v>
       </c>
       <c r="D165" t="s">
-        <v>18</v>
+        <v>322</v>
       </c>
       <c r="E165" t="s">
-        <v>337</v>
+        <v>146</v>
       </c>
       <c r="G165" t="e">
         <f>VLOOKUP(B165, Sheet2!$A$1:$B$65, 2, FALSE)</f>
@@ -5375,10 +5461,10 @@
         <v>165</v>
       </c>
       <c r="B166" t="s">
-        <v>266</v>
+        <v>268</v>
       </c>
       <c r="C166" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="D166" t="s">
         <v>18</v>
@@ -5386,9 +5472,9 @@
       <c r="E166" t="s">
         <v>337</v>
       </c>
-      <c r="G166" t="str">
+      <c r="G166" t="e">
         <f>VLOOKUP(B166, Sheet2!$A$1:$B$65, 2, FALSE)</f>
-        <v>Central Services</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="167" spans="1:7">
@@ -5396,20 +5482,20 @@
         <v>166</v>
       </c>
       <c r="B167" t="s">
-        <v>271</v>
+        <v>266</v>
       </c>
       <c r="C167" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="D167" t="s">
-        <v>322</v>
+        <v>18</v>
       </c>
       <c r="E167" t="s">
         <v>337</v>
       </c>
-      <c r="G167" t="e">
+      <c r="G167" t="str">
         <f>VLOOKUP(B167, Sheet2!$A$1:$B$65, 2, FALSE)</f>
-        <v>#N/A</v>
+        <v>Central Services</v>
       </c>
     </row>
     <row r="168" spans="1:7">
@@ -5417,16 +5503,16 @@
         <v>167</v>
       </c>
       <c r="B168" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="C168" t="s">
-        <v>166</v>
+        <v>270</v>
       </c>
       <c r="D168" t="s">
         <v>322</v>
       </c>
-      <c r="E168" s="3" t="s">
-        <v>330</v>
+      <c r="E168" t="s">
+        <v>337</v>
       </c>
       <c r="G168" t="e">
         <f>VLOOKUP(B168, Sheet2!$A$1:$B$65, 2, FALSE)</f>
@@ -5438,13 +5524,13 @@
         <v>168</v>
       </c>
       <c r="B169" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="C169" t="s">
-        <v>273</v>
+        <v>166</v>
       </c>
       <c r="D169" t="s">
-        <v>18</v>
+        <v>322</v>
       </c>
       <c r="E169" s="3" t="s">
         <v>330</v>
@@ -5459,20 +5545,20 @@
         <v>169</v>
       </c>
       <c r="B170" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="C170" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="D170" t="s">
-        <v>322</v>
+        <v>18</v>
       </c>
       <c r="E170" s="3" t="s">
         <v>330</v>
       </c>
-      <c r="G170" t="str">
+      <c r="G170" t="e">
         <f>VLOOKUP(B170, Sheet2!$A$1:$B$65, 2, FALSE)</f>
-        <v>Helpful Resources</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="171" spans="1:7">
@@ -5480,10 +5566,10 @@
         <v>170</v>
       </c>
       <c r="B171" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="C171" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="D171" t="s">
         <v>322</v>
@@ -5501,10 +5587,10 @@
         <v>171</v>
       </c>
       <c r="B172" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="C172" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="D172" t="s">
         <v>322</v>
@@ -5512,9 +5598,9 @@
       <c r="E172" s="3" t="s">
         <v>330</v>
       </c>
-      <c r="G172" t="e">
+      <c r="G172" t="str">
         <f>VLOOKUP(B172, Sheet2!$A$1:$B$65, 2, FALSE)</f>
-        <v>#N/A</v>
+        <v>Helpful Resources</v>
       </c>
     </row>
     <row r="173" spans="1:7">
@@ -5522,20 +5608,19 @@
         <v>172</v>
       </c>
       <c r="B173" t="s">
-        <v>143</v>
+        <v>280</v>
       </c>
       <c r="C173" t="s">
-        <v>142</v>
+        <v>279</v>
       </c>
       <c r="D173" t="s">
-        <v>18</v>
+        <v>322</v>
       </c>
       <c r="E173" s="3" t="s">
         <v>330</v>
       </c>
-      <c r="G173" t="e">
-        <f>VLOOKUP(B173, Sheet2!$A$1:$B$65, 2, FALSE)</f>
-        <v>#N/A</v>
+      <c r="G173" t="s">
+        <v>383</v>
       </c>
     </row>
     <row r="174" spans="1:7">
@@ -5543,10 +5628,10 @@
         <v>173</v>
       </c>
       <c r="B174" t="s">
-        <v>193</v>
+        <v>143</v>
       </c>
       <c r="C174" t="s">
-        <v>194</v>
+        <v>142</v>
       </c>
       <c r="D174" t="s">
         <v>18</v>
@@ -5564,20 +5649,20 @@
         <v>174</v>
       </c>
       <c r="B175" t="s">
-        <v>282</v>
+        <v>193</v>
       </c>
       <c r="C175" t="s">
-        <v>281</v>
+        <v>194</v>
       </c>
       <c r="D175" t="s">
-        <v>322</v>
+        <v>18</v>
       </c>
       <c r="E175" s="3" t="s">
         <v>330</v>
       </c>
-      <c r="G175" t="str">
+      <c r="G175" t="e">
         <f>VLOOKUP(B175, Sheet2!$A$1:$B$65, 2, FALSE)</f>
-        <v>Life at SLAC</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="176" spans="1:7">
@@ -5585,20 +5670,20 @@
         <v>175</v>
       </c>
       <c r="B176" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="C176" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="D176" t="s">
         <v>322</v>
       </c>
       <c r="E176" s="3" t="s">
-        <v>331</v>
-      </c>
-      <c r="G176" t="e">
+        <v>330</v>
+      </c>
+      <c r="G176" t="str">
         <f>VLOOKUP(B176, Sheet2!$A$1:$B$65, 2, FALSE)</f>
-        <v>#N/A</v>
+        <v>Life at SLAC</v>
       </c>
     </row>
     <row r="177" spans="1:7">
@@ -5606,10 +5691,10 @@
         <v>176</v>
       </c>
       <c r="B177" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="C177" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="D177" t="s">
         <v>322</v>
@@ -5617,9 +5702,8 @@
       <c r="E177" s="3" t="s">
         <v>331</v>
       </c>
-      <c r="G177" t="e">
-        <f>VLOOKUP(B177, Sheet2!$A$1:$B$65, 2, FALSE)</f>
-        <v>#N/A</v>
+      <c r="G177" t="s">
+        <v>403</v>
       </c>
     </row>
     <row r="178" spans="1:7">
@@ -5627,10 +5711,10 @@
         <v>177</v>
       </c>
       <c r="B178" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="C178" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="D178" t="s">
         <v>322</v>
@@ -5648,10 +5732,10 @@
         <v>178</v>
       </c>
       <c r="B179" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="C179" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="D179" t="s">
         <v>322</v>
@@ -5669,20 +5753,20 @@
         <v>179</v>
       </c>
       <c r="B180" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="C180" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="D180" t="s">
         <v>322</v>
       </c>
       <c r="E180" s="3" t="s">
-        <v>332</v>
-      </c>
-      <c r="G180" t="str">
+        <v>331</v>
+      </c>
+      <c r="G180" t="e">
         <f>VLOOKUP(B180, Sheet2!$A$1:$B$65, 2, FALSE)</f>
-        <v>HR Services &amp; Benefits</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="181" spans="1:7">
@@ -5690,10 +5774,10 @@
         <v>180</v>
       </c>
       <c r="B181" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="C181" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="D181" t="s">
         <v>322</v>
@@ -5703,7 +5787,7 @@
       </c>
       <c r="G181" t="str">
         <f>VLOOKUP(B181, Sheet2!$A$1:$B$65, 2, FALSE)</f>
-        <v>Policies &amp; Procedures</v>
+        <v>HR Services &amp; Benefits</v>
       </c>
     </row>
     <row r="182" spans="1:7">
@@ -5711,20 +5795,20 @@
         <v>181</v>
       </c>
       <c r="B182" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="C182" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="D182" t="s">
         <v>322</v>
       </c>
       <c r="E182" s="3" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="G182" t="str">
         <f>VLOOKUP(B182, Sheet2!$A$1:$B$65, 2, FALSE)</f>
-        <v>Life at SLAC</v>
+        <v>Policies &amp; Procedures</v>
       </c>
     </row>
     <row r="183" spans="1:7">
@@ -5732,10 +5816,10 @@
         <v>182</v>
       </c>
       <c r="B183" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="C183" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="D183" t="s">
         <v>322</v>
@@ -5743,9 +5827,9 @@
       <c r="E183" s="3" t="s">
         <v>333</v>
       </c>
-      <c r="G183" t="e">
+      <c r="G183" t="str">
         <f>VLOOKUP(B183, Sheet2!$A$1:$B$65, 2, FALSE)</f>
-        <v>#N/A</v>
+        <v>Life at SLAC</v>
       </c>
     </row>
     <row r="184" spans="1:7">
@@ -5753,10 +5837,10 @@
         <v>183</v>
       </c>
       <c r="B184" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="C184" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="D184" t="s">
         <v>322</v>
@@ -5764,9 +5848,9 @@
       <c r="E184" s="3" t="s">
         <v>333</v>
       </c>
-      <c r="G184" t="str">
+      <c r="G184" t="e">
         <f>VLOOKUP(B184, Sheet2!$A$1:$B$65, 2, FALSE)</f>
-        <v>Life at SLAC</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="185" spans="1:7">
@@ -5774,10 +5858,10 @@
         <v>184</v>
       </c>
       <c r="B185" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="C185" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="D185" t="s">
         <v>322</v>
@@ -5785,9 +5869,9 @@
       <c r="E185" s="3" t="s">
         <v>333</v>
       </c>
-      <c r="G185" t="e">
+      <c r="G185" t="str">
         <f>VLOOKUP(B185, Sheet2!$A$1:$B$65, 2, FALSE)</f>
-        <v>#N/A</v>
+        <v>Life at SLAC</v>
       </c>
     </row>
     <row r="186" spans="1:7">
@@ -5795,10 +5879,10 @@
         <v>185</v>
       </c>
       <c r="B186" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="C186" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="D186" t="s">
         <v>322</v>
@@ -5806,9 +5890,8 @@
       <c r="E186" s="3" t="s">
         <v>333</v>
       </c>
-      <c r="G186" t="e">
-        <f>VLOOKUP(B186, Sheet2!$A$1:$B$65, 2, FALSE)</f>
-        <v>#N/A</v>
+      <c r="G186" t="s">
+        <v>383</v>
       </c>
     </row>
     <row r="187" spans="1:7">
@@ -5816,10 +5899,10 @@
         <v>186</v>
       </c>
       <c r="B187" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="C187" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="D187" t="s">
         <v>322</v>
@@ -5827,9 +5910,8 @@
       <c r="E187" s="3" t="s">
         <v>333</v>
       </c>
-      <c r="G187" t="e">
-        <f>VLOOKUP(B187, Sheet2!$A$1:$B$65, 2, FALSE)</f>
-        <v>#N/A</v>
+      <c r="G187" t="s">
+        <v>383</v>
       </c>
     </row>
     <row r="188" spans="1:7">
@@ -5837,10 +5919,10 @@
         <v>187</v>
       </c>
       <c r="B188" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="C188" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="D188" t="s">
         <v>322</v>
@@ -5858,20 +5940,19 @@
         <v>188</v>
       </c>
       <c r="B189" t="s">
-        <v>274</v>
+        <v>308</v>
       </c>
       <c r="C189" t="s">
-        <v>273</v>
+        <v>307</v>
       </c>
       <c r="D189" t="s">
-        <v>18</v>
+        <v>322</v>
       </c>
       <c r="E189" s="3" t="s">
         <v>333</v>
       </c>
-      <c r="G189" t="e">
-        <f>VLOOKUP(B189, Sheet2!$A$1:$B$65, 2, FALSE)</f>
-        <v>#N/A</v>
+      <c r="G189" t="s">
+        <v>342</v>
       </c>
     </row>
     <row r="190" spans="1:7">
@@ -5879,13 +5960,13 @@
         <v>189</v>
       </c>
       <c r="B190" t="s">
-        <v>310</v>
+        <v>274</v>
       </c>
       <c r="C190" t="s">
-        <v>309</v>
+        <v>273</v>
       </c>
       <c r="D190" t="s">
-        <v>322</v>
+        <v>18</v>
       </c>
       <c r="E190" s="3" t="s">
         <v>333</v>
@@ -5900,10 +5981,10 @@
         <v>190</v>
       </c>
       <c r="B191" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="C191" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="D191" t="s">
         <v>322</v>
@@ -5911,9 +5992,9 @@
       <c r="E191" s="3" t="s">
         <v>333</v>
       </c>
-      <c r="G191" t="str">
+      <c r="G191" t="e">
         <f>VLOOKUP(B191, Sheet2!$A$1:$B$65, 2, FALSE)</f>
-        <v>Life at SLAC</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="192" spans="1:7">
@@ -5921,26 +6002,603 @@
         <v>191</v>
       </c>
       <c r="B192" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="C192" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="D192" t="s">
-        <v>18</v>
+        <v>322</v>
       </c>
       <c r="E192" s="3" t="s">
         <v>333</v>
       </c>
       <c r="G192" t="str">
         <f>VLOOKUP(B192, Sheet2!$A$1:$B$65, 2, FALSE)</f>
+        <v>Life at SLAC</v>
+      </c>
+    </row>
+    <row r="193" spans="1:7">
+      <c r="A193">
+        <v>192</v>
+      </c>
+      <c r="B193" t="s">
+        <v>314</v>
+      </c>
+      <c r="C193" t="s">
+        <v>313</v>
+      </c>
+      <c r="D193" t="s">
+        <v>18</v>
+      </c>
+      <c r="E193" s="3" t="s">
+        <v>333</v>
+      </c>
+      <c r="G193" t="str">
+        <f>VLOOKUP(B193, Sheet2!$A$1:$B$65, 2, FALSE)</f>
         <v>HR Services &amp; Benefits</v>
       </c>
     </row>
+    <row r="194" spans="1:7">
+      <c r="A194">
+        <v>193</v>
+      </c>
+      <c r="B194" t="s">
+        <v>386</v>
+      </c>
+      <c r="C194" t="s">
+        <v>387</v>
+      </c>
+      <c r="D194" t="s">
+        <v>322</v>
+      </c>
+      <c r="E194" s="3" t="s">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="195" spans="1:7">
+      <c r="A195">
+        <v>194</v>
+      </c>
+      <c r="B195" t="s">
+        <v>389</v>
+      </c>
+      <c r="C195" t="s">
+        <v>390</v>
+      </c>
+      <c r="D195" t="s">
+        <v>322</v>
+      </c>
+      <c r="E195" s="3" t="s">
+        <v>388</v>
+      </c>
+      <c r="G195" t="s">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="196" spans="1:7">
+      <c r="A196">
+        <v>195</v>
+      </c>
+      <c r="B196" t="s">
+        <v>391</v>
+      </c>
+      <c r="C196" t="s">
+        <v>392</v>
+      </c>
+      <c r="D196" t="s">
+        <v>322</v>
+      </c>
+      <c r="E196" s="3" t="s">
+        <v>388</v>
+      </c>
+      <c r="G196" t="s">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="197" spans="1:7">
+      <c r="A197">
+        <v>196</v>
+      </c>
+      <c r="B197" t="s">
+        <v>380</v>
+      </c>
+      <c r="C197" t="s">
+        <v>394</v>
+      </c>
+      <c r="D197" t="s">
+        <v>18</v>
+      </c>
+      <c r="E197" s="3" t="s">
+        <v>388</v>
+      </c>
+      <c r="G197" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="198" spans="1:7">
+      <c r="A198">
+        <v>197</v>
+      </c>
+      <c r="B198" t="s">
+        <v>347</v>
+      </c>
+      <c r="C198" t="s">
+        <v>395</v>
+      </c>
+      <c r="D198" t="s">
+        <v>18</v>
+      </c>
+      <c r="E198" s="3" t="s">
+        <v>388</v>
+      </c>
+      <c r="G198" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="199" spans="1:7">
+      <c r="A199">
+        <v>198</v>
+      </c>
+      <c r="B199" t="s">
+        <v>370</v>
+      </c>
+      <c r="C199" t="s">
+        <v>396</v>
+      </c>
+      <c r="D199" t="s">
+        <v>18</v>
+      </c>
+      <c r="E199" s="3" t="s">
+        <v>388</v>
+      </c>
+      <c r="G199" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="200" spans="1:7">
+      <c r="A200">
+        <v>199</v>
+      </c>
+      <c r="B200" t="s">
+        <v>371</v>
+      </c>
+      <c r="C200" t="s">
+        <v>397</v>
+      </c>
+      <c r="D200" t="s">
+        <v>322</v>
+      </c>
+      <c r="E200" s="3" t="s">
+        <v>388</v>
+      </c>
+      <c r="G200" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="201" spans="1:7">
+      <c r="A201">
+        <v>200</v>
+      </c>
+      <c r="B201" t="s">
+        <v>375</v>
+      </c>
+      <c r="C201" t="s">
+        <v>398</v>
+      </c>
+      <c r="D201" t="s">
+        <v>322</v>
+      </c>
+      <c r="E201" s="3" t="s">
+        <v>388</v>
+      </c>
+      <c r="G201" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="202" spans="1:7">
+      <c r="A202">
+        <v>201</v>
+      </c>
+      <c r="B202" t="s">
+        <v>376</v>
+      </c>
+      <c r="C202" t="s">
+        <v>399</v>
+      </c>
+      <c r="D202" t="s">
+        <v>322</v>
+      </c>
+      <c r="E202" s="3" t="s">
+        <v>388</v>
+      </c>
+      <c r="G202" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="203" spans="1:7">
+      <c r="A203">
+        <v>202</v>
+      </c>
+      <c r="B203" t="s">
+        <v>345</v>
+      </c>
+      <c r="C203" t="s">
+        <v>400</v>
+      </c>
+      <c r="D203" t="s">
+        <v>18</v>
+      </c>
+      <c r="E203" s="3" t="s">
+        <v>388</v>
+      </c>
+      <c r="G203" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="204" spans="1:7">
+      <c r="A204">
+        <v>203</v>
+      </c>
+      <c r="B204" t="s">
+        <v>360</v>
+      </c>
+      <c r="C204" t="s">
+        <v>401</v>
+      </c>
+      <c r="D204" t="s">
+        <v>18</v>
+      </c>
+      <c r="E204" s="3" t="s">
+        <v>388</v>
+      </c>
+      <c r="G204" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="205" spans="1:7">
+      <c r="A205">
+        <v>204</v>
+      </c>
+      <c r="B205" t="s">
+        <v>379</v>
+      </c>
+      <c r="C205" t="s">
+        <v>402</v>
+      </c>
+      <c r="D205" t="s">
+        <v>18</v>
+      </c>
+      <c r="E205" s="3" t="s">
+        <v>388</v>
+      </c>
+      <c r="G205" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="206" spans="1:7">
+      <c r="A206">
+        <v>205</v>
+      </c>
+      <c r="B206" t="s">
+        <v>349</v>
+      </c>
+      <c r="C206" t="s">
+        <v>404</v>
+      </c>
+      <c r="D206" t="s">
+        <v>322</v>
+      </c>
+      <c r="E206" s="3" t="s">
+        <v>388</v>
+      </c>
+      <c r="G206" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="207" spans="1:7">
+      <c r="A207">
+        <v>206</v>
+      </c>
+      <c r="B207" t="s">
+        <v>381</v>
+      </c>
+      <c r="C207" t="s">
+        <v>405</v>
+      </c>
+      <c r="D207" t="s">
+        <v>322</v>
+      </c>
+      <c r="E207" s="3" t="s">
+        <v>388</v>
+      </c>
+      <c r="G207" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="208" spans="1:7">
+      <c r="A208">
+        <v>207</v>
+      </c>
+      <c r="B208" t="s">
+        <v>356</v>
+      </c>
+      <c r="C208" t="s">
+        <v>406</v>
+      </c>
+      <c r="D208" t="s">
+        <v>322</v>
+      </c>
+      <c r="E208" s="3" t="s">
+        <v>388</v>
+      </c>
+      <c r="G208" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="209" spans="1:7">
+      <c r="A209">
+        <v>208</v>
+      </c>
+      <c r="B209" t="s">
+        <v>361</v>
+      </c>
+      <c r="C209" t="s">
+        <v>407</v>
+      </c>
+      <c r="D209" t="s">
+        <v>322</v>
+      </c>
+      <c r="E209" s="3" t="s">
+        <v>388</v>
+      </c>
+      <c r="G209" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="210" spans="1:7">
+      <c r="A210">
+        <v>209</v>
+      </c>
+      <c r="B210" t="s">
+        <v>365</v>
+      </c>
+      <c r="C210" t="s">
+        <v>408</v>
+      </c>
+      <c r="D210" t="s">
+        <v>322</v>
+      </c>
+      <c r="E210" s="3" t="s">
+        <v>388</v>
+      </c>
+      <c r="G210" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="211" spans="1:7">
+      <c r="A211">
+        <v>210</v>
+      </c>
+      <c r="B211" t="s">
+        <v>369</v>
+      </c>
+      <c r="C211" t="s">
+        <v>409</v>
+      </c>
+      <c r="D211" t="s">
+        <v>322</v>
+      </c>
+      <c r="E211" s="3" t="s">
+        <v>388</v>
+      </c>
+      <c r="G211" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="212" spans="1:7">
+      <c r="A212">
+        <v>211</v>
+      </c>
+      <c r="B212" t="s">
+        <v>310</v>
+      </c>
+      <c r="C212" t="s">
+        <v>411</v>
+      </c>
+      <c r="D212" t="s">
+        <v>322</v>
+      </c>
+      <c r="E212" s="3" t="s">
+        <v>388</v>
+      </c>
+      <c r="G212" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="213" spans="1:7">
+      <c r="A213">
+        <v>212</v>
+      </c>
+      <c r="B213" t="s">
+        <v>382</v>
+      </c>
+      <c r="C213" t="s">
+        <v>412</v>
+      </c>
+      <c r="D213" t="s">
+        <v>322</v>
+      </c>
+      <c r="E213" s="3" t="s">
+        <v>388</v>
+      </c>
+      <c r="G213" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="214" spans="1:7">
+      <c r="A214">
+        <v>213</v>
+      </c>
+      <c r="B214" t="s">
+        <v>355</v>
+      </c>
+      <c r="C214" t="s">
+        <v>413</v>
+      </c>
+      <c r="D214" t="s">
+        <v>322</v>
+      </c>
+      <c r="E214" s="3" t="s">
+        <v>388</v>
+      </c>
+      <c r="G214" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="215" spans="1:7">
+      <c r="A215">
+        <v>214</v>
+      </c>
+      <c r="B215" t="s">
+        <v>415</v>
+      </c>
+      <c r="C215" t="s">
+        <v>414</v>
+      </c>
+      <c r="D215" t="s">
+        <v>322</v>
+      </c>
+      <c r="E215" s="3" t="s">
+        <v>388</v>
+      </c>
+      <c r="G215" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="216" spans="1:7">
+      <c r="A216">
+        <v>215</v>
+      </c>
+      <c r="B216" t="s">
+        <v>358</v>
+      </c>
+      <c r="C216" t="s">
+        <v>416</v>
+      </c>
+      <c r="D216" t="s">
+        <v>322</v>
+      </c>
+      <c r="E216" s="3" t="s">
+        <v>388</v>
+      </c>
+      <c r="G216" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="217" spans="1:7">
+      <c r="A217">
+        <v>216</v>
+      </c>
+      <c r="B217" t="s">
+        <v>359</v>
+      </c>
+      <c r="C217" t="s">
+        <v>417</v>
+      </c>
+      <c r="D217" t="s">
+        <v>322</v>
+      </c>
+      <c r="E217" s="3" t="s">
+        <v>388</v>
+      </c>
+      <c r="G217" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="218" spans="1:7">
+      <c r="A218">
+        <v>217</v>
+      </c>
+      <c r="B218" t="s">
+        <v>362</v>
+      </c>
+      <c r="C218" t="s">
+        <v>418</v>
+      </c>
+      <c r="D218" t="s">
+        <v>322</v>
+      </c>
+      <c r="E218" s="3" t="s">
+        <v>388</v>
+      </c>
+      <c r="G218" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="219" spans="1:7">
+      <c r="A219">
+        <v>218</v>
+      </c>
+      <c r="B219" t="s">
+        <v>265</v>
+      </c>
+      <c r="C219" t="s">
+        <v>419</v>
+      </c>
+      <c r="D219" t="s">
+        <v>322</v>
+      </c>
+      <c r="E219" s="3" t="s">
+        <v>388</v>
+      </c>
+      <c r="G219" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="220" spans="1:7">
+      <c r="A220">
+        <v>219</v>
+      </c>
+      <c r="B220" t="s">
+        <v>420</v>
+      </c>
+      <c r="C220" t="s">
+        <v>421</v>
+      </c>
+      <c r="D220" t="s">
+        <v>322</v>
+      </c>
+      <c r="E220" s="3" t="s">
+        <v>388</v>
+      </c>
+      <c r="G220" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="221" spans="1:7">
+      <c r="A221">
+        <v>220</v>
+      </c>
+      <c r="B221" t="s">
+        <v>378</v>
+      </c>
+      <c r="C221" t="s">
+        <v>422</v>
+      </c>
+      <c r="D221" t="s">
+        <v>322</v>
+      </c>
+      <c r="E221" s="3" t="s">
+        <v>388</v>
+      </c>
+      <c r="G221" t="s">
+        <v>343</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:G192"/>
+  <autoFilter ref="A1:G193"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>